<commit_message>
Initial commit: Synergy M&A model
</commit_message>
<xml_diff>
--- a/mna_deals.xlsx
+++ b/mna_deals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romaincalfati/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romaincalfati/Documents/HEC M1/Finance application/Python Stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB8C984-D6C9-1E45-85ED-228DAF74238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E21F11-E2BF-DD47-A97C-3CD396A2F26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Deal Name</t>
   </si>
@@ -43,53 +43,50 @@
     <t>Duration (years)</t>
   </si>
   <si>
-    <t>Microsoft-LinkedIn</t>
-  </si>
-  <si>
-    <t>Amazon-WholeFoods</t>
-  </si>
-  <si>
-    <t>Facebook-WhatsApp</t>
-  </si>
-  <si>
-    <t>Salesforce-Slack</t>
-  </si>
-  <si>
-    <t>Google-Fitbit</t>
-  </si>
-  <si>
-    <t>Disney-Fox</t>
-  </si>
-  <si>
-    <t>Intel-Altera</t>
-  </si>
-  <si>
-    <t>CVS-Aetna</t>
-  </si>
-  <si>
-    <t>Dell-EMC</t>
-  </si>
-  <si>
-    <t>AT&amp;T-TimeWarner</t>
-  </si>
-  <si>
-    <t>Tech</t>
-  </si>
-  <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
-    <t>Media</t>
+    <t>The data in these tables are examples that do not necessarily reflect reality.</t>
+  </si>
+  <si>
+    <t>Railroads</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>Canadian National - KCS</t>
+  </si>
+  <si>
+    <t>Union Pacific - Western Rail</t>
+  </si>
+  <si>
+    <t>Norfolk Southern - Southern Railway</t>
+  </si>
+  <si>
+    <t>Kansas City Southern - CP</t>
+  </si>
+  <si>
+    <t>Genesee &amp; Wyoming - Rail America</t>
+  </si>
+  <si>
+    <t>CSX - NS</t>
+  </si>
+  <si>
+    <t>BNSF Railway - Grand Trunk</t>
+  </si>
+  <si>
+    <t>Canadian Pacifi - Illinois Central</t>
+  </si>
+  <si>
+    <t>MTR - KCR</t>
+  </si>
+  <si>
+    <t>CNR - CSR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +102,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -141,10 +151,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,15 +463,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,237 +494,262 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>4.5</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
+        <v>4.8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2">
-        <v>1000</v>
+        <v>850</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3">
+        <v>5.5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>900</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3.9</v>
+      </c>
+      <c r="D4">
+        <v>1.7</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>400</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>5.2</v>
       </c>
-      <c r="D3">
-        <v>2.7</v>
-      </c>
-      <c r="E3">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>300</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>3.8</v>
-      </c>
-      <c r="D4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E4">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>600</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>6.1</v>
-      </c>
       <c r="D5">
-        <v>2.2000000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="E5">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5">
-        <v>450</v>
+        <v>750</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D6">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D7">
+        <v>3.2</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>1800</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>4.9000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="D8">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="E8">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="G8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>2.9</v>
+      </c>
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>900</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D10">
+        <v>2.9</v>
+      </c>
+      <c r="E10">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>600</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
-        <v>2.5</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>17</v>
-      </c>
-      <c r="F9">
-        <v>700</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>5.6</v>
-      </c>
-      <c r="D10">
-        <v>3.5</v>
-      </c>
-      <c r="E10">
-        <v>23</v>
-      </c>
-      <c r="F10">
-        <v>2000</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>6.8</v>
+        <v>5.4</v>
       </c>
       <c r="D11">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="E11">
         <v>28</v>
       </c>
       <c r="F11">
-        <v>1500</v>
+        <v>950</v>
       </c>
       <c r="G11">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I6:S6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>